<commit_message>
axios desde front, resolviendo errores
</commit_message>
<xml_diff>
--- a/formatoSimple.xlsx
+++ b/formatoSimple.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="33">
   <si>
     <t xml:space="preserve">NOMBRE EMPRESA</t>
   </si>
@@ -65,16 +65,7 @@
     <t xml:space="preserve">NOTA</t>
   </si>
   <si>
-    <t xml:space="preserve">Nike</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nike.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E-Learning</t>
-  </si>
-  <si>
-    <t xml:space="preserve">USA</t>
+    <t xml:space="preserve">royal</t>
   </si>
   <si>
     <t xml:space="preserve">mario</t>
@@ -86,7 +77,7 @@
     <t xml:space="preserve">+323423432</t>
   </si>
   <si>
-    <t xml:space="preserve">mario@nike.com</t>
+    <t xml:space="preserve">mario@eltiempo.com</t>
   </si>
   <si>
     <t xml:space="preserve">appointmentscheduled</t>
@@ -101,10 +92,31 @@
     <t xml:space="preserve">HOLAMUNDO</t>
   </si>
   <si>
-    <t xml:space="preserve">Nike 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mario2@gmail.com</t>
+    <t xml:space="preserve">royal2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GFF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FFF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DFDF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FGFF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GFDGFD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">royal3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">roya4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">roya5</t>
   </si>
   <si>
     <t xml:space="preserve">PERRRI ME LO PELA</t>
@@ -117,11 +129,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -175,12 +188,20 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -230,7 +251,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -260,6 +281,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -344,15 +369,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I5" activeCellId="0" sqref="I5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I10" activeCellId="0" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="21.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="23.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.47"/>
@@ -409,94 +437,284 @@
       <c r="A2" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="C2" s="5"/>
+      <c r="E2" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="F2" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="G2" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="H2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="I2" s="5" t="s">
         <v>19</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>22</v>
       </c>
       <c r="J2" s="0" t="n">
         <v>1000</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="L2" s="7" t="n">
         <v>46846311</v>
       </c>
       <c r="M2" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="N2" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="N2" s="0" t="s">
+      <c r="C3" s="5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="s">
+      <c r="D3" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="8" t="s">
+      <c r="E3" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="H3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="I3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="J3" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="K3" s="0" t="s">
         <v>20</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="J3" s="8" t="n">
-        <v>1000</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>23</v>
       </c>
       <c r="L3" s="7" t="n">
         <v>46846311</v>
       </c>
-      <c r="M3" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="N3" s="8" t="s">
-        <v>25</v>
-      </c>
+      <c r="M3" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="N3" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="G4" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="L4" s="7" t="n">
+        <v>46846311</v>
+      </c>
+      <c r="M4" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="N4" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="H5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="K5" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="L5" s="7" t="n">
+        <v>46846311</v>
+      </c>
+      <c r="M5" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="N5" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="H6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K6" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="L6" s="7" t="n">
+        <v>46846311</v>
+      </c>
+      <c r="M6" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="N6" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="H7" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="L7" s="7" t="n">
+        <v>46846311</v>
+      </c>
+      <c r="M7" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="N7" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C8" s="5"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="5"/>
+      <c r="L8" s="7"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C9" s="5"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="5"/>
+      <c r="L9" s="7"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C10" s="5"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="5"/>
+      <c r="L10" s="8"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C11" s="5"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="5"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C12" s="5"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="5"/>
+      <c r="L12" s="8"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C13" s="5"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="5"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C14" s="5"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="5"/>
+      <c r="L14" s="8"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C15" s="5"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="5"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="9"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C16" s="5"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="5"/>
+      <c r="L16" s="8"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C17" s="5"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="5"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="9"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C18" s="5"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="5"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="9"/>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="9"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="9"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1" display="mario@nike.com"/>
-    <hyperlink ref="H3" r:id="rId2" display="mario2@gmail.com"/>
+    <hyperlink ref="H2" r:id="rId1" display="mario@eltiempo.com"/>
+    <hyperlink ref="H3" r:id="rId2" display="mario@eltiempo.com"/>
+    <hyperlink ref="H4" r:id="rId3" display="mario@eltiempo.com"/>
+    <hyperlink ref="H5" r:id="rId4" display="mario@eltiempo.com"/>
+    <hyperlink ref="H6" r:id="rId5" display="mario@eltiempo.com"/>
+    <hyperlink ref="H7" r:id="rId6" display="mario@eltiempo.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -515,7 +733,7 @@
   </sheetPr>
   <dimension ref="C9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -526,13 +744,13 @@
   <sheetData>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
agregando validaciones en front y numero de empresas registradas
</commit_message>
<xml_diff>
--- a/formatoSimple.xlsx
+++ b/formatoSimple.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="36">
   <si>
     <t xml:space="preserve">NOMBRE EMPRESA</t>
   </si>
@@ -65,7 +65,16 @@
     <t xml:space="preserve">NOTA</t>
   </si>
   <si>
-    <t xml:space="preserve">royal</t>
+    <t xml:space="preserve">ROA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">roa.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alimentos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">col</t>
   </si>
   <si>
     <t xml:space="preserve">mario</t>
@@ -77,7 +86,7 @@
     <t xml:space="preserve">+323423432</t>
   </si>
   <si>
-    <t xml:space="preserve">mario@eltiempo.com</t>
+    <t xml:space="preserve">mario@roa.com</t>
   </si>
   <si>
     <t xml:space="preserve">appointmentscheduled</t>
@@ -92,31 +101,31 @@
     <t xml:space="preserve">HOLAMUNDO</t>
   </si>
   <si>
-    <t xml:space="preserve">royal2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GFF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FFF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DFDF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FGFF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GFDGFD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">royal3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">roya4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">roya5</t>
+    <t xml:space="preserve">ROA 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mario@roa2.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ROA 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZEV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zev.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZEV1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZEV2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZEV3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZEV4</t>
   </si>
   <si>
     <t xml:space="preserve">PERRRI ME LO PELA</t>
@@ -129,7 +138,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -202,11 +211,6 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -251,7 +255,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -281,10 +285,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -372,7 +372,7 @@
   <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I10" activeCellId="0" sqref="I10"/>
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -437,284 +437,444 @@
       <c r="A2" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="5"/>
+      <c r="B2" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>17</v>
+      </c>
       <c r="E2" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="J2" s="0" t="n">
         <v>1000</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="L2" s="7" t="n">
         <v>46846311</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="E3" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>18</v>
-      </c>
       <c r="I3" s="5" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="J3" s="0" t="n">
         <v>1000</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="L3" s="7" t="n">
         <v>46846311</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="N3" s="0" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="5"/>
+        <v>28</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>19</v>
+      </c>
       <c r="G4" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="J4" s="0" t="n">
         <v>1000</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="L4" s="7" t="n">
         <v>46846311</v>
       </c>
       <c r="M4" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="N4" s="0" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="5"/>
+      <c r="C5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>20</v>
+      </c>
       <c r="H5" s="6" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="J5" s="0" t="n">
         <v>1000</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="L5" s="7" t="n">
         <v>46846311</v>
       </c>
       <c r="M5" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="N5" s="0" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="5"/>
+      <c r="C6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>20</v>
+      </c>
       <c r="H6" s="6" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>19</v>
+        <v>22</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>1000</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="L6" s="7" t="n">
         <v>46846311</v>
       </c>
       <c r="M6" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="N6" s="0" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" s="5"/>
+        <v>32</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>20</v>
+      </c>
       <c r="H7" s="6" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>19</v>
+        <v>22</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="K7" s="0" t="s">
+        <v>23</v>
       </c>
       <c r="L7" s="7" t="n">
         <v>46846311</v>
       </c>
       <c r="M7" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="N7" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="I8" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C8" s="5"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="5"/>
-      <c r="L8" s="7"/>
+      <c r="J8" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="K8" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="L8" s="7" t="n">
+        <v>46846311</v>
+      </c>
+      <c r="M8" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="N8" s="0" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C9" s="5"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="5"/>
-      <c r="L9" s="7"/>
+      <c r="A9" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="K9" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="L9" s="7" t="n">
+        <v>46846311</v>
+      </c>
+      <c r="M9" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="N9" s="0" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="5"/>
       <c r="H10" s="6"/>
       <c r="I10" s="5"/>
-      <c r="L10" s="8"/>
+      <c r="L10" s="7"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="5"/>
       <c r="H11" s="6"/>
       <c r="I11" s="5"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="9"/>
-      <c r="N11" s="9"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="5"/>
       <c r="H12" s="6"/>
       <c r="I12" s="5"/>
-      <c r="L12" s="8"/>
+      <c r="L12" s="7"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="5"/>
       <c r="H13" s="6"/>
       <c r="I13" s="5"/>
-      <c r="L13" s="8"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="9"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="5"/>
       <c r="H14" s="6"/>
       <c r="I14" s="5"/>
-      <c r="L14" s="8"/>
+      <c r="L14" s="7"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="5"/>
       <c r="H15" s="6"/>
       <c r="I15" s="5"/>
-      <c r="L15" s="8"/>
-      <c r="M15" s="9"/>
-      <c r="N15" s="9"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="5"/>
       <c r="H16" s="6"/>
       <c r="I16" s="5"/>
-      <c r="L16" s="8"/>
+      <c r="L16" s="7"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C17" s="5"/>
       <c r="H17" s="6"/>
       <c r="I17" s="5"/>
-      <c r="L17" s="8"/>
-      <c r="M17" s="9"/>
-      <c r="N17" s="9"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="5"/>
       <c r="H18" s="6"/>
       <c r="I18" s="5"/>
-      <c r="L18" s="8"/>
-      <c r="M18" s="9"/>
-      <c r="N18" s="9"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="8"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="9"/>
-      <c r="B19" s="9"/>
+      <c r="A19" s="8"/>
+      <c r="B19" s="8"/>
       <c r="C19" s="5"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
       <c r="H19" s="6"/>
       <c r="I19" s="5"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="9"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
       <c r="L19" s="7"/>
-      <c r="M19" s="9"/>
-      <c r="N19" s="9"/>
+      <c r="M19" s="8"/>
+      <c r="N19" s="8"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1" display="mario@eltiempo.com"/>
-    <hyperlink ref="H3" r:id="rId2" display="mario@eltiempo.com"/>
-    <hyperlink ref="H4" r:id="rId3" display="mario@eltiempo.com"/>
-    <hyperlink ref="H5" r:id="rId4" display="mario@eltiempo.com"/>
-    <hyperlink ref="H6" r:id="rId5" display="mario@eltiempo.com"/>
-    <hyperlink ref="H7" r:id="rId6" display="mario@eltiempo.com"/>
+    <hyperlink ref="H2" r:id="rId1" display="mario@roa.com"/>
+    <hyperlink ref="H3" r:id="rId2" display="mario@roa2.com"/>
+    <hyperlink ref="H4" r:id="rId3" display="mario@roa2.com"/>
+    <hyperlink ref="H5" r:id="rId4" display="mario@roa2.com"/>
+    <hyperlink ref="H6" r:id="rId5" display="mario@roa2.com"/>
+    <hyperlink ref="H7" r:id="rId6" display="mario@roa2.com"/>
+    <hyperlink ref="H8" r:id="rId7" display="mario@roa2.com"/>
+    <hyperlink ref="H9" r:id="rId8" display="mario@roa2.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -744,7 +904,7 @@
   <sheetData>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>